<commit_message>
Evolução na parte de GC
Agora com os Titles testados conectados ao Google Sheet. Informações da planilha e chave de API na aba de notas dentro da branch
</commit_message>
<xml_diff>
--- a/GC/TesteTarjaScript.xlsx
+++ b/GC/TesteTarjaScript.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julourei\Desktop\VMIX\Scripting\GC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julourei\Desktop\VMIX\GitHub\automacaoVmix\GC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3CFA3A-E2FB-4013-AA22-62FF34D7C5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4668C9-78E2-4A14-B620-D69CEF5F7CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{43685A29-456B-4182-A182-0F27D065DDDA}"/>
   </bookViews>
@@ -41,11 +41,14 @@
   <connection id="2" xr16:uid="{C195882F-C66E-43C8-ADFE-837B81A92FC3}" name="mapaTarja1" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\julourei\Desktop\VMIX\Scripting\GC\mapaTarja.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
+  <connection id="3" xr16:uid="{8230ECF8-576C-4143-87D9-E6DBC4B7AE08}" name="mapaTarja2" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\julourei\Desktop\VMIX\GitHub\automacaoVmix\GC\mapaTarja.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>Headline</t>
   </si>
@@ -62,28 +65,31 @@
     <t>teste2</t>
   </si>
   <si>
+    <t>teste4</t>
+  </si>
+  <si>
+    <t>teste5</t>
+  </si>
+  <si>
+    <t>teste6</t>
+  </si>
+  <si>
+    <t>teste7</t>
+  </si>
+  <si>
+    <t>teste8</t>
+  </si>
+  <si>
+    <t>teste9</t>
+  </si>
+  <si>
+    <t>teste10</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
     <t>teste3</t>
-  </si>
-  <si>
-    <t>teste4</t>
-  </si>
-  <si>
-    <t>teste5</t>
-  </si>
-  <si>
-    <t>teste6</t>
-  </si>
-  <si>
-    <t>teste7</t>
-  </si>
-  <si>
-    <t>teste8</t>
-  </si>
-  <si>
-    <t>teste9</t>
-  </si>
-  <si>
-    <t>teste10</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -152,6 +157,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -169,7 +175,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema2">
+  <Schema ID="Schema3">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="testeTitle0">
         <xsd:complexType>
@@ -188,24 +194,24 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="2" Name="testeTitle0_Mapa" RootElement="testeTitle0" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
+  <Map ID="3" Name="testeTitle0_Mapa" RootElement="testeTitle0" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6CD4D83D-A2F5-4FC5-83D9-823C0CC1A889}" name="Tabela4" displayName="Tabela4" ref="A1:C11" tableType="xml" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" connectionId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6CD4D83D-A2F5-4FC5-83D9-823C0CC1A889}" name="Tabela4" displayName="Tabela4" ref="A1:C11" tableType="xml" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" connectionId="3">
   <autoFilter ref="A1:C11" xr:uid="{6CD4D83D-A2F5-4FC5-83D9-823C0CC1A889}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{287D8138-E88A-49FA-B085-4F2977D2AD94}" uniqueName="pagina" name="Pagina" dataDxfId="4">
-      <xmlColumnPr mapId="2" xpath="/testeTitle0/texto/pagina" xmlDataType="integer"/>
+    <tableColumn id="1" xr3:uid="{287D8138-E88A-49FA-B085-4F2977D2AD94}" uniqueName="pagina" name="Pagina" dataDxfId="2">
+      <xmlColumnPr mapId="3" xpath="/testeTitle0/texto/pagina" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EB251902-F9A8-4E09-91A1-75783CBB2A64}" uniqueName="headline" name="Headline" dataDxfId="3">
-      <xmlColumnPr mapId="2" xpath="/testeTitle0/texto/headline" xmlDataType="string"/>
+    <tableColumn id="2" xr3:uid="{EB251902-F9A8-4E09-91A1-75783CBB2A64}" uniqueName="headline" name="Headline" dataDxfId="1">
+      <xmlColumnPr mapId="3" xpath="/testeTitle0/texto/headline" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4A02E1C6-2816-487F-9F65-81D333D60E81}" uniqueName="description" name="Description" dataDxfId="2">
-      <xmlColumnPr mapId="2" xpath="/testeTitle0/texto/description" xmlDataType="string"/>
+    <tableColumn id="3" xr3:uid="{4A02E1C6-2816-487F-9F65-81D333D60E81}" uniqueName="description" name="Description" dataDxfId="0">
+      <xmlColumnPr mapId="3" xpath="/testeTitle0/texto/description" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -512,17 +518,17 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -549,7 +555,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>4</v>
@@ -560,10 +566,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -571,10 +577,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -582,10 +588,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -593,10 +599,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -604,10 +610,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -615,10 +621,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -626,10 +632,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -637,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>